<commit_message>
* Changed colour correction from LUT to proper gamma correction function
</commit_message>
<xml_diff>
--- a/ColourMap.xlsx
+++ b/ColourMap.xlsx
@@ -358,15 +358,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E257"/>
+  <dimension ref="A1:F257"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -380,7 +380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -394,8 +394,12 @@
         <f>LOOKUP(D2,$B$2:$B$257,$A$2:$A$257)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <f>((D2/255)^(2.2))*255</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -409,8 +413,12 @@
         <f t="shared" ref="E3:E66" si="0">LOOKUP(D3,$B$2:$B$257,$A$2:$A$257)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="1">((D3/255)^(2.2))*255</f>
+        <v>1.2946482346687486E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -424,8 +432,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>5.9486411898552185E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -439,8 +451,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>1.451505025660923E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -454,8 +470,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>2.7332777397017179E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -469,8 +489,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>4.4656614263271797E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -484,8 +508,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>6.669365740986527E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -499,8 +527,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>9.3619748803065381E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -513,8 +545,12 @@
       <c r="E10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0.12558846573381535</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -527,8 +563,12 @@
       <c r="E11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0.16273662475259065</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -541,8 +581,12 @@
       <c r="E12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0.20518791737582984</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -555,8 +599,12 @@
       <c r="E13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0.25305544753895298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -569,8 +617,12 @@
       <c r="E14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0.30644357822179252</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -583,8 +635,12 @@
       <c r="E15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0.36544932036632533</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -597,8 +653,12 @@
       <c r="E16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0.43016340578126744</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -611,8 +671,12 @@
       <c r="E17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>0.50067113441609978</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -625,8 +689,12 @@
       <c r="E18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>0.57705305598014034</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -639,8 +707,12 @@
       <c r="E19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>0.65938552703971276</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -653,8 +725,12 @@
       <c r="E20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>0.74774117260428274</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -667,8 +743,12 @@
       <c r="E21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>0.84218927316092829</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -681,8 +761,12 @@
       <c r="E22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>0.94279609261953246</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -696,8 +780,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>1.0496251587871024</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -711,8 +799,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>1.1627375052441353</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -726,8 +818,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>1.2821918814981617</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -741,8 +837,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>1.4080449368111134</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -756,8 +856,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>1.5403513819867032</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -771,8 +875,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>1.6791641325583297</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -786,8 +894,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>1.8245344361661224</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -801,8 +913,12 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>1.9765119864034544</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -816,8 +932,12 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>2.1351450250128887</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -831,8 +951,12 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>2.3004804339930933</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -846,8 +970,12 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>2.4725638189228474</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -861,8 +989,12 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>2.6514395846015972</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -876,8 +1008,12 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>2.8371510039377275</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -891,8 +1027,12 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>3.0297402808774847</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -906,8 +1046,12 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>3.2292486080534371</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -921,8 +1065,12 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>3.4357162197363751</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -936,8 +1084,12 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>3.6491824405954363</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -951,8 +1103,12 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <f t="shared" si="1"/>
+        <v>3.869685730704425</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -966,8 +1122,12 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <f t="shared" si="1"/>
+        <v>4.0972637271761529</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -981,8 +1141,12 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <f t="shared" si="1"/>
+        <v>4.3319532827587617</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -996,8 +1160,12 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <f t="shared" si="1"/>
+        <v>4.5737905016873102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1011,8 +1179,12 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <f t="shared" si="1"/>
+        <v>4.8228107730489835</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1026,8 +1198,12 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <f t="shared" si="1"/>
+        <v>5.0790488018903597</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1041,8 +1217,12 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <f t="shared" si="1"/>
+        <v>5.3425386382691791</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1056,8 +1236,12 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <f t="shared" si="1"/>
+        <v>5.6133137044308175</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1071,8 +1255,12 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <f t="shared" si="1"/>
+        <v>5.8914068202699683</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -1086,8 +1274,12 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <f t="shared" si="1"/>
+        <v>6.1768502272212302</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -1101,8 +1293,12 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <f t="shared" si="1"/>
+        <v>6.469675610707319</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -1116,8 +1312,12 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <f t="shared" si="1"/>
+        <v>6.7699141212605918</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -1131,8 +1331,12 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <f t="shared" si="1"/>
+        <v>7.0775963944221392</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -1146,8 +1350,12 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <f t="shared" si="1"/>
+        <v>7.3927525695124938</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -1161,8 +1369,12 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <f t="shared" si="1"/>
+        <v>7.7154123073591085</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -1176,8 +1388,12 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <f t="shared" si="1"/>
+        <v>8.0456048070577442</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -1191,8 +1407,12 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <f t="shared" si="1"/>
+        <v>8.3833588218378754</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -1206,8 +1426,12 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <f t="shared" si="1"/>
+        <v>8.7287026740958957</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -1221,8 +1445,12 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <f t="shared" si="1"/>
+        <v>9.0816642696542864</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -1236,8 +1464,12 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <f t="shared" si="1"/>
+        <v>9.4422711112998492</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -1251,8 +1483,12 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <f t="shared" si="1"/>
+        <v>9.8105503116496298</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -1266,8 +1502,12 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <f t="shared" si="1"/>
+        <v>10.186528605389025</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -1281,8 +1521,12 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <f t="shared" si="1"/>
+        <v>10.57023236092293</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -1296,8 +1540,12 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <f t="shared" si="1"/>
+        <v>10.961687591477565</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -1311,8 +1559,12 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <f t="shared" si="1"/>
+        <v>11.360919965687454</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -1326,8 +1578,12 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <f t="shared" si="1"/>
+        <v>11.767954817699492</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -1341,8 +1597,12 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <f t="shared" si="1"/>
+        <v>12.182817156823514</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -1353,11 +1613,15 @@
         <v>65</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E130" si="1">LOOKUP(D67,$B$2:$B$257,$A$2:$A$257)</f>
+        <f t="shared" ref="E67:E130" si="2">LOOKUP(D67,$B$2:$B$257,$A$2:$A$257)</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <f t="shared" ref="F67:F130" si="3">((D67/255)^(2.2))*255</f>
+        <v>12.605531676756529</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -1368,11 +1632,15 @@
         <v>66</v>
       </c>
       <c r="E68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <f t="shared" si="3"/>
+        <v>13.03612276440581</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -1383,11 +1651,15 @@
         <v>67</v>
       </c>
       <c r="E69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <f t="shared" si="3"/>
+        <v>13.474614508334151</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -1398,11 +1670,15 @@
         <v>68</v>
       </c>
       <c r="E70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <f t="shared" si="3"/>
+        <v>13.921030706848883</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -1413,11 +1689,15 @@
         <v>69</v>
       </c>
       <c r="E71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <f t="shared" si="3"/>
+        <v>14.375394875754836</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
@@ -1428,11 +1708,15 @@
         <v>70</v>
       </c>
       <c r="E72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <f t="shared" si="3"/>
+        <v>14.837730255789783</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -1443,11 +1727,15 @@
         <v>71</v>
       </c>
       <c r="E73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <f t="shared" si="3"/>
+        <v>15.308059819759871</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -1458,11 +1746,15 @@
         <v>72</v>
       </c>
       <c r="E74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <f t="shared" si="3"/>
+        <v>15.786406279391212</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
@@ -1473,11 +1765,15 @@
         <v>73</v>
       </c>
       <c r="E75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75">
+        <f t="shared" si="3"/>
+        <v>16.272792091912699</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
@@ -1488,11 +1784,15 @@
         <v>74</v>
       </c>
       <c r="E76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76">
+        <f t="shared" si="3"/>
+        <v>16.767239466384176</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
@@ -1503,11 +1803,15 @@
         <v>75</v>
       </c>
       <c r="E77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77">
+        <f t="shared" si="3"/>
+        <v>17.269770369783203</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
@@ -1518,11 +1822,15 @@
         <v>76</v>
       </c>
       <c r="E78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F78">
+        <f t="shared" si="3"/>
+        <v>17.780406532862692</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
@@ -1533,11 +1841,15 @@
         <v>77</v>
       </c>
       <c r="E79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79">
+        <f t="shared" si="3"/>
+        <v>18.299169455790963</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
@@ -1548,11 +1860,15 @@
         <v>78</v>
       </c>
       <c r="E80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80">
+        <f t="shared" si="3"/>
+        <v>18.826080413585075</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -1563,11 +1879,15 @@
         <v>79</v>
       </c>
       <c r="E81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F81">
+        <f t="shared" si="3"/>
+        <v>19.36116046134752</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
@@ -1578,11 +1898,15 @@
         <v>80</v>
       </c>
       <c r="E82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F82">
+        <f t="shared" si="3"/>
+        <v>19.904430439315984</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
@@ -1593,11 +1917,15 @@
         <v>81</v>
       </c>
       <c r="E83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F83">
+        <f t="shared" si="3"/>
+        <v>20.455910977734835</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
@@ -1608,11 +1936,15 @@
         <v>82</v>
       </c>
       <c r="E84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F84">
+        <f t="shared" si="3"/>
+        <v>21.015622501557111</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
@@ -1623,11 +1955,15 @@
         <v>83</v>
       </c>
       <c r="E85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F85">
+        <f t="shared" si="3"/>
+        <v>21.583585234984511</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
@@ -1638,11 +1974,15 @@
         <v>84</v>
       </c>
       <c r="E86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F86">
+        <f t="shared" si="3"/>
+        <v>22.159819205853378</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
@@ -1653,11 +1993,15 @@
         <v>85</v>
       </c>
       <c r="E87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F87">
+        <f t="shared" si="3"/>
+        <v>22.744344249873194</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
@@ -1668,11 +2012,15 @@
         <v>86</v>
       </c>
       <c r="E88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F88">
+        <f t="shared" si="3"/>
+        <v>23.337180014724467</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
@@ -1683,11 +2031,15 @@
         <v>87</v>
       </c>
       <c r="E89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F89">
+        <f t="shared" si="3"/>
+        <v>23.938345964022332</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
@@ -1698,11 +2050,15 @@
         <v>88</v>
       </c>
       <c r="E90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F90">
+        <f t="shared" si="3"/>
+        <v>24.547861381151627</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
@@ -1713,11 +2069,15 @@
         <v>89</v>
       </c>
       <c r="E91">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F91">
+        <f t="shared" si="3"/>
+        <v>25.165745372979078</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
@@ -1728,11 +2088,15 @@
         <v>90</v>
       </c>
       <c r="E92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F92">
+        <f t="shared" si="3"/>
+        <v>25.792016873447974</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
@@ -1743,11 +2107,15 @@
         <v>91</v>
       </c>
       <c r="E93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F93">
+        <f t="shared" si="3"/>
+        <v>26.426694647060032</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
@@ -1758,11 +2126,15 @@
         <v>92</v>
       </c>
       <c r="E94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F94">
+        <f t="shared" si="3"/>
+        <v>27.069797292249703</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
@@ -1773,11 +2145,15 @@
         <v>93</v>
       </c>
       <c r="E95">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F95">
+        <f t="shared" si="3"/>
+        <v>27.721343244654832</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
@@ -1788,11 +2164,15 @@
         <v>94</v>
       </c>
       <c r="E96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F96">
+        <f t="shared" si="3"/>
+        <v>28.381350780288361</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
@@ -1803,11 +2183,15 @@
         <v>95</v>
       </c>
       <c r="E97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F97">
+        <f t="shared" si="3"/>
+        <v>29.049838018614842</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
@@ -1818,11 +2202,15 @@
         <v>96</v>
       </c>
       <c r="E98">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F98">
+        <f t="shared" si="3"/>
+        <v>29.726822925535746</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
@@ -1833,11 +2221,15 @@
         <v>97</v>
       </c>
       <c r="E99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F99">
+        <f t="shared" si="3"/>
+        <v>30.412323316287093</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
@@ -1848,11 +2240,15 @@
         <v>98</v>
       </c>
       <c r="E100">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F100">
+        <f t="shared" si="3"/>
+        <v>31.10635685825298</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
@@ -1863,11 +2259,15 @@
         <v>99</v>
       </c>
       <c r="E101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F101">
+        <f t="shared" si="3"/>
+        <v>31.808941073698076</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>100</v>
       </c>
@@ -1878,11 +2278,15 @@
         <v>100</v>
       </c>
       <c r="E102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F102">
+        <f t="shared" si="3"/>
+        <v>32.520093342422641</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>101</v>
       </c>
@@ -1893,11 +2297,15 @@
         <v>101</v>
       </c>
       <c r="E103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F103">
+        <f t="shared" si="3"/>
+        <v>33.239830904342305</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>102</v>
       </c>
@@ -1908,11 +2316,15 @@
         <v>102</v>
       </c>
       <c r="E104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F104">
+        <f t="shared" si="3"/>
+        <v>33.968170861996427</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>103</v>
       </c>
@@ -1923,11 +2335,15 @@
         <v>103</v>
       </c>
       <c r="E105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F105">
+        <f t="shared" si="3"/>
+        <v>34.705130182986629</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>104</v>
       </c>
@@ -1938,11 +2354,15 @@
         <v>104</v>
       </c>
       <c r="E106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F106">
+        <f t="shared" si="3"/>
+        <v>35.450725702349139</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>105</v>
       </c>
@@ -1953,11 +2373,15 @@
         <v>105</v>
       </c>
       <c r="E107">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F107">
+        <f t="shared" si="3"/>
+        <v>36.204974124862559</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>106</v>
       </c>
@@ -1968,11 +2392,15 @@
         <v>106</v>
       </c>
       <c r="E108">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F108">
+        <f t="shared" si="3"/>
+        <v>36.967892027293878</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>107</v>
       </c>
@@ -1983,11 +2411,15 @@
         <v>107</v>
       </c>
       <c r="E109">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F109">
+        <f t="shared" si="3"/>
+        <v>37.739495860584718</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>108</v>
       </c>
@@ -1998,11 +2430,15 @@
         <v>108</v>
       </c>
       <c r="E110">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F110">
+        <f t="shared" si="3"/>
+        <v>38.519801951980206</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>109</v>
       </c>
@@ -2013,11 +2449,15 @@
         <v>109</v>
       </c>
       <c r="E111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F111">
+        <f t="shared" si="3"/>
+        <v>39.308826507102118</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>110</v>
       </c>
@@ -2028,11 +2468,15 @@
         <v>110</v>
       </c>
       <c r="E112">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F112">
+        <f t="shared" si="3"/>
+        <v>40.106585611968718</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>111</v>
       </c>
@@ -2043,11 +2487,15 @@
         <v>111</v>
       </c>
       <c r="E113">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F113">
+        <f t="shared" si="3"/>
+        <v>40.913095234962597</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>112</v>
       </c>
@@ -2058,11 +2506,15 @@
         <v>112</v>
       </c>
       <c r="E114">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F114">
+        <f t="shared" si="3"/>
+        <v>41.728371228748919</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>113</v>
       </c>
@@ -2073,11 +2525,15 @@
         <v>113</v>
       </c>
       <c r="E115">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F115">
+        <f t="shared" si="3"/>
+        <v>42.552429332145202</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>114</v>
       </c>
@@ -2088,11 +2544,15 @@
         <v>114</v>
       </c>
       <c r="E116">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F116">
+        <f t="shared" si="3"/>
+        <v>43.385285171944659</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>115</v>
       </c>
@@ -2103,11 +2563,15 @@
         <v>115</v>
       </c>
       <c r="E117">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F117">
+        <f t="shared" si="3"/>
+        <v>44.226954264694434</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>116</v>
       </c>
@@ -2118,11 +2582,15 @@
         <v>116</v>
       </c>
       <c r="E118">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F118">
+        <f t="shared" si="3"/>
+        <v>45.077452018430336</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>117</v>
       </c>
@@ -2133,11 +2601,15 @@
         <v>117</v>
       </c>
       <c r="E119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F119">
+        <f t="shared" si="3"/>
+        <v>45.936793734369537</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>118</v>
       </c>
@@ -2148,11 +2620,15 @@
         <v>118</v>
       </c>
       <c r="E120">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F120">
+        <f t="shared" si="3"/>
+        <v>46.80499460856246</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>119</v>
       </c>
@@ -2163,11 +2639,15 @@
         <v>119</v>
       </c>
       <c r="E121">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F121">
+        <f t="shared" si="3"/>
+        <v>47.68206973350528</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>120</v>
       </c>
@@ -2178,11 +2658,15 @@
         <v>120</v>
       </c>
       <c r="E122">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F122">
+        <f t="shared" si="3"/>
+        <v>48.568034099714374</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>121</v>
       </c>
@@ -2193,11 +2677,15 @@
         <v>121</v>
       </c>
       <c r="E123">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F123">
+        <f t="shared" si="3"/>
+        <v>49.462902597263742</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>122</v>
       </c>
@@ -2208,11 +2696,15 @@
         <v>122</v>
       </c>
       <c r="E124">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F124">
+        <f t="shared" si="3"/>
+        <v>50.36669001728675</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>123</v>
       </c>
@@ -2223,11 +2715,15 @@
         <v>123</v>
       </c>
       <c r="E125">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>51</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F125">
+        <f t="shared" si="3"/>
+        <v>51.279411053443148</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>124</v>
       </c>
@@ -2238,11 +2734,15 @@
         <v>124</v>
       </c>
       <c r="E126">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F126">
+        <f t="shared" si="3"/>
+        <v>52.20108030335259</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>125</v>
       </c>
@@ -2253,11 +2753,15 @@
         <v>125</v>
       </c>
       <c r="E127">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>53</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F127">
+        <f t="shared" si="3"/>
+        <v>53.131712269995688</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>126</v>
       </c>
@@ -2268,11 +2772,15 @@
         <v>126</v>
       </c>
       <c r="E128">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F128">
+        <f t="shared" si="3"/>
+        <v>54.071321363083364</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>127</v>
       </c>
@@ -2283,11 +2791,15 @@
         <v>127</v>
       </c>
       <c r="E129">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>55</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F129">
+        <f t="shared" si="3"/>
+        <v>55.019921900395723</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>128</v>
       </c>
@@ -2298,11 +2810,15 @@
         <v>128</v>
       </c>
       <c r="E130">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>56</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F130">
+        <f t="shared" si="3"/>
+        <v>55.97752810909131</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>129</v>
       </c>
@@ -2313,11 +2829,15 @@
         <v>129</v>
       </c>
       <c r="E131">
-        <f t="shared" ref="E131:E194" si="2">LOOKUP(D131,$B$2:$B$257,$A$2:$A$257)</f>
+        <f t="shared" ref="E131:E194" si="4">LOOKUP(D131,$B$2:$B$257,$A$2:$A$257)</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F131">
+        <f t="shared" ref="F131:F194" si="5">((D131/255)^(2.2))*255</f>
+        <v>56.944154126987492</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>130</v>
       </c>
@@ -2328,11 +2848,15 @@
         <v>130</v>
       </c>
       <c r="E132">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>58</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F132">
+        <f t="shared" si="5"/>
+        <v>57.919814003812974</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>131</v>
       </c>
@@ -2343,11 +2867,15 @@
         <v>131</v>
       </c>
       <c r="E133">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>59</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F133">
+        <f t="shared" si="5"/>
+        <v>58.904521702433193</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>132</v>
       </c>
@@ -2358,11 +2886,15 @@
         <v>132</v>
       </c>
       <c r="E134">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F134">
+        <f t="shared" si="5"/>
+        <v>59.898291100049448</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>133</v>
       </c>
@@ -2373,11 +2905,15 @@
         <v>133</v>
       </c>
       <c r="E135">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>61</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F135">
+        <f t="shared" si="5"/>
+        <v>60.901135989372314</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>134</v>
       </c>
@@ -2388,11 +2924,15 @@
         <v>134</v>
       </c>
       <c r="E136">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>62</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F136">
+        <f t="shared" si="5"/>
+        <v>61.913070079770499</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>135</v>
       </c>
@@ -2403,11 +2943,15 @@
         <v>135</v>
       </c>
       <c r="E137">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>63</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F137">
+        <f t="shared" si="5"/>
+        <v>62.934106998395364</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>136</v>
       </c>
@@ -2418,11 +2962,15 @@
         <v>136</v>
       </c>
       <c r="E138">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>64</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F138">
+        <f t="shared" si="5"/>
+        <v>63.964260291282102</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>137</v>
       </c>
@@ -2433,11 +2981,15 @@
         <v>137</v>
       </c>
       <c r="E139">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>65</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F139">
+        <f t="shared" si="5"/>
+        <v>65.003543424428202</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>138</v>
       </c>
@@ -2448,11 +3000,15 @@
         <v>138</v>
       </c>
       <c r="E140">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>66</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F140">
+        <f t="shared" si="5"/>
+        <v>66.051969784849561</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>139</v>
       </c>
@@ -2463,11 +3019,15 @@
         <v>139</v>
       </c>
       <c r="E141">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>67</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F141">
+        <f t="shared" si="5"/>
+        <v>67.109552681615355</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>140</v>
       </c>
@@ -2478,11 +3038,15 @@
         <v>140</v>
       </c>
       <c r="E142">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>68</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F142">
+        <f t="shared" si="5"/>
+        <v>68.176305346861852</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>141</v>
       </c>
@@ -2493,11 +3057,15 @@
         <v>141</v>
       </c>
       <c r="E143">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>69</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F143">
+        <f t="shared" si="5"/>
+        <v>69.25224093678564</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>142</v>
       </c>
@@ -2508,11 +3076,15 @@
         <v>142</v>
       </c>
       <c r="E144">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F144">
+        <f t="shared" si="5"/>
+        <v>70.337372532617508</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>143</v>
       </c>
@@ -2523,11 +3095,15 @@
         <v>143</v>
       </c>
       <c r="E145">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>71</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F145">
+        <f t="shared" si="5"/>
+        <v>71.431713141576651</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>144</v>
       </c>
@@ -2538,11 +3114,15 @@
         <v>144</v>
       </c>
       <c r="E146">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>73</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F146">
+        <f t="shared" si="5"/>
+        <v>72.535275697806256</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>145</v>
       </c>
@@ -2553,11 +3133,15 @@
         <v>145</v>
       </c>
       <c r="E147">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>74</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F147">
+        <f t="shared" si="5"/>
+        <v>73.648073063290738</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>146</v>
       </c>
@@ -2568,11 +3152,15 @@
         <v>146</v>
       </c>
       <c r="E148">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>75</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F148">
+        <f t="shared" si="5"/>
+        <v>74.770118028755505</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>147</v>
       </c>
@@ -2583,11 +3171,15 @@
         <v>147</v>
       </c>
       <c r="E149">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>76</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F149">
+        <f t="shared" si="5"/>
+        <v>75.90142331454885</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>148</v>
       </c>
@@ -2598,11 +3190,15 @@
         <v>148</v>
       </c>
       <c r="E150">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>77</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F150">
+        <f t="shared" si="5"/>
+        <v>77.04200157150747</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>149</v>
       </c>
@@ -2613,11 +3209,15 @@
         <v>149</v>
       </c>
       <c r="E151">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>78</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F151">
+        <f t="shared" si="5"/>
+        <v>78.191865381805187</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>150</v>
       </c>
@@ -2628,11 +3228,15 @@
         <v>150</v>
       </c>
       <c r="E152">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>79</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F152">
+        <f t="shared" si="5"/>
+        <v>79.351027259786008</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>151</v>
       </c>
@@ -2643,11 +3247,15 @@
         <v>151</v>
       </c>
       <c r="E153">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>81</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F153">
+        <f t="shared" si="5"/>
+        <v>80.519499652781249</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>152</v>
       </c>
@@ -2658,11 +3266,15 @@
         <v>152</v>
       </c>
       <c r="E154">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>82</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F154">
+        <f t="shared" si="5"/>
+        <v>81.69729494191165</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>153</v>
       </c>
@@ -2673,11 +3285,15 @@
         <v>153</v>
       </c>
       <c r="E155">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>83</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F155">
+        <f t="shared" si="5"/>
+        <v>82.884425442874445</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>154</v>
       </c>
@@ -2688,11 +3304,15 @@
         <v>154</v>
       </c>
       <c r="E156">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>84</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F156">
+        <f t="shared" si="5"/>
+        <v>84.080903406716288</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>155</v>
       </c>
@@ -2703,11 +3323,15 @@
         <v>155</v>
       </c>
       <c r="E157">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>85</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F157">
+        <f t="shared" si="5"/>
+        <v>85.286741020591762</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>156</v>
       </c>
@@ -2718,11 +3342,15 @@
         <v>156</v>
       </c>
       <c r="E158">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>87</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F158">
+        <f t="shared" si="5"/>
+        <v>86.501950408508321</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>157</v>
       </c>
@@ -2733,11 +3361,15 @@
         <v>157</v>
       </c>
       <c r="E159">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>88</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F159">
+        <f t="shared" si="5"/>
+        <v>87.726543632057641</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>158</v>
       </c>
@@ -2748,11 +3380,15 @@
         <v>158</v>
       </c>
       <c r="E160">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>89</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F160">
+        <f t="shared" si="5"/>
+        <v>88.960532691134148</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>159</v>
       </c>
@@ -2763,11 +3399,15 @@
         <v>159</v>
       </c>
       <c r="E161">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F161">
+        <f t="shared" si="5"/>
+        <v>90.203929524640529</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>160</v>
       </c>
@@ -2778,11 +3418,15 @@
         <v>160</v>
       </c>
       <c r="E162">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>92</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F162">
+        <f t="shared" si="5"/>
+        <v>91.456746011180712</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>161</v>
       </c>
@@ -2793,11 +3437,15 @@
         <v>161</v>
       </c>
       <c r="E163">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>93</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F163">
+        <f t="shared" si="5"/>
+        <v>92.718993969741064</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>162</v>
       </c>
@@ -2808,11 +3456,15 @@
         <v>162</v>
       </c>
       <c r="E164">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F164">
+        <f t="shared" si="5"/>
+        <v>93.990685160359206</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>163</v>
       </c>
@@ -2823,11 +3475,15 @@
         <v>163</v>
       </c>
       <c r="E165">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>95</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F165">
+        <f t="shared" si="5"/>
+        <v>95.271831284781499</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>164</v>
       </c>
@@ -2838,11 +3494,15 @@
         <v>164</v>
       </c>
       <c r="E166">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>97</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F166">
+        <f t="shared" si="5"/>
+        <v>96.56244398710929</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>165</v>
       </c>
@@ -2853,11 +3513,15 @@
         <v>165</v>
       </c>
       <c r="E167">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F167">
+        <f t="shared" si="5"/>
+        <v>97.862534854433676</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>166</v>
       </c>
@@ -2868,11 +3532,15 @@
         <v>166</v>
       </c>
       <c r="E168">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>99</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F168">
+        <f t="shared" si="5"/>
+        <v>99.172115417460006</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>167</v>
       </c>
@@ -2883,11 +3551,15 @@
         <v>167</v>
       </c>
       <c r="E169">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>101</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F169">
+        <f t="shared" si="5"/>
+        <v>100.49119715112138</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>168</v>
       </c>
@@ -2898,11 +3570,15 @@
         <v>168</v>
       </c>
       <c r="E170">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>102</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F170">
+        <f t="shared" si="5"/>
+        <v>101.81979147518196</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>169</v>
       </c>
@@ -2913,11 +3589,15 @@
         <v>169</v>
       </c>
       <c r="E171">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>103</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F171">
+        <f t="shared" si="5"/>
+        <v>103.15790975483027</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>170</v>
       </c>
@@ -2928,11 +3608,15 @@
         <v>170</v>
       </c>
       <c r="E172">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>105</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F172">
+        <f t="shared" si="5"/>
+        <v>104.50556330126246</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>171</v>
       </c>
@@ -2943,11 +3627,15 @@
         <v>171</v>
       </c>
       <c r="E173">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>106</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F173">
+        <f t="shared" si="5"/>
+        <v>105.86276337225615</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>172</v>
       </c>
@@ -2958,11 +3646,15 @@
         <v>172</v>
       </c>
       <c r="E174">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>107</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F174">
+        <f t="shared" si="5"/>
+        <v>107.22952117273472</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>173</v>
       </c>
@@ -2973,11 +3665,15 @@
         <v>173</v>
       </c>
       <c r="E175">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>109</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F175">
+        <f t="shared" si="5"/>
+        <v>108.60584785532215</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>174</v>
       </c>
@@ -2988,11 +3684,15 @@
         <v>174</v>
       </c>
       <c r="E176">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>110</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F176">
+        <f t="shared" si="5"/>
+        <v>109.99175452088946</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>175</v>
       </c>
@@ -3003,11 +3703,15 @@
         <v>175</v>
       </c>
       <c r="E177">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>112</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F177">
+        <f t="shared" si="5"/>
+        <v>111.38725221909165</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>176</v>
       </c>
@@ -3018,11 +3722,15 @@
         <v>176</v>
       </c>
       <c r="E178">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>113</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F178">
+        <f t="shared" si="5"/>
+        <v>112.79235194889647</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>177</v>
       </c>
@@ -3033,11 +3741,15 @@
         <v>177</v>
       </c>
       <c r="E179">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>114</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F179">
+        <f t="shared" si="5"/>
+        <v>114.20706465910455</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>178</v>
       </c>
@@ -3048,11 +3760,15 @@
         <v>178</v>
       </c>
       <c r="E180">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>116</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F180">
+        <f t="shared" si="5"/>
+        <v>115.63140124886128</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>179</v>
       </c>
@@ -3063,11 +3779,15 @@
         <v>179</v>
       </c>
       <c r="E181">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>117</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F181">
+        <f t="shared" si="5"/>
+        <v>117.06537256816083</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>180</v>
       </c>
@@ -3078,11 +3798,15 @@
         <v>180</v>
       </c>
       <c r="E182">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>118</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F182">
+        <f t="shared" si="5"/>
+        <v>118.50898941834184</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>181</v>
       </c>
@@ -3093,11 +3817,15 @@
         <v>181</v>
       </c>
       <c r="E183">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>120</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F183">
+        <f t="shared" si="5"/>
+        <v>119.96226255257569</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>182</v>
       </c>
@@ -3108,11 +3836,15 @@
         <v>182</v>
       </c>
       <c r="E184">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>122</v>
       </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F184">
+        <f t="shared" si="5"/>
+        <v>121.42520267634725</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>183</v>
       </c>
@@ -3123,11 +3855,15 @@
         <v>183</v>
       </c>
       <c r="E185">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>123</v>
       </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F185">
+        <f t="shared" si="5"/>
+        <v>122.89782044792794</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>184</v>
       </c>
@@ -3138,11 +3874,15 @@
         <v>184</v>
       </c>
       <c r="E186">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>125</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F186">
+        <f t="shared" si="5"/>
+        <v>124.3801264788417</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>185</v>
       </c>
@@ -3153,11 +3893,15 @@
         <v>185</v>
       </c>
       <c r="E187">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>126</v>
       </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F187">
+        <f t="shared" si="5"/>
+        <v>125.87213133432378</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>186</v>
       </c>
@@ -3168,11 +3912,15 @@
         <v>186</v>
       </c>
       <c r="E188">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>128</v>
       </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F188">
+        <f t="shared" si="5"/>
+        <v>127.37384553377269</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>187</v>
       </c>
@@ -3183,11 +3931,15 @@
         <v>187</v>
       </c>
       <c r="E189">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>129</v>
       </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F189">
+        <f t="shared" si="5"/>
+        <v>128.88527955119508</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>188</v>
       </c>
@@ -3198,11 +3950,15 @@
         <v>188</v>
       </c>
       <c r="E190">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>131</v>
       </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F190">
+        <f t="shared" si="5"/>
+        <v>130.40644381564422</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>189</v>
       </c>
@@ -3213,11 +3969,15 @@
         <v>189</v>
       </c>
       <c r="E191">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>132</v>
       </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F191">
+        <f t="shared" si="5"/>
+        <v>131.93734871165174</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>190</v>
       </c>
@@ -3228,11 +3988,15 @@
         <v>190</v>
       </c>
       <c r="E192">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>134</v>
       </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F192">
+        <f t="shared" si="5"/>
+        <v>133.4780045796528</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>191</v>
       </c>
@@ -3243,11 +4007,15 @@
         <v>191</v>
       </c>
       <c r="E193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>135</v>
       </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F193">
+        <f t="shared" si="5"/>
+        <v>135.02842171640569</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>192</v>
       </c>
@@ -3258,11 +4026,15 @@
         <v>192</v>
       </c>
       <c r="E194">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>137</v>
       </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F194">
+        <f t="shared" si="5"/>
+        <v>136.58861037540424</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>193</v>
       </c>
@@ -3273,11 +4045,15 @@
         <v>193</v>
       </c>
       <c r="E195">
-        <f t="shared" ref="E195:E257" si="3">LOOKUP(D195,$B$2:$B$257,$A$2:$A$257)</f>
+        <f t="shared" ref="E195:E257" si="6">LOOKUP(D195,$B$2:$B$257,$A$2:$A$257)</f>
         <v>138</v>
       </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F195">
+        <f t="shared" ref="F195:F257" si="7">((D195/255)^(2.2))*255</f>
+        <v>138.15858076728492</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>194</v>
       </c>
@@ -3288,11 +4064,15 @@
         <v>194</v>
       </c>
       <c r="E196">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>140</v>
       </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F196">
+        <f t="shared" si="7"/>
+        <v>139.73834306022783</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>195</v>
       </c>
@@ -3303,11 +4083,15 @@
         <v>195</v>
       </c>
       <c r="E197">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>142</v>
       </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F197">
+        <f t="shared" si="7"/>
+        <v>141.32790738035172</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>196</v>
       </c>
@@ -3318,11 +4102,15 @@
         <v>196</v>
       </c>
       <c r="E198">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>143</v>
       </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F198">
+        <f t="shared" si="7"/>
+        <v>142.9272838121037</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>197</v>
       </c>
@@ -3333,11 +4121,15 @@
         <v>197</v>
       </c>
       <c r="E199">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>144</v>
       </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F199">
+        <f t="shared" si="7"/>
+        <v>144.5364823986427</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>198</v>
       </c>
@@ -3348,11 +4140,15 @@
         <v>198</v>
       </c>
       <c r="E200">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>146</v>
       </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F200">
+        <f t="shared" si="7"/>
+        <v>146.15551314221844</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>199</v>
       </c>
@@ -3363,11 +4159,15 @@
         <v>199</v>
       </c>
       <c r="E201">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>148</v>
       </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F201">
+        <f t="shared" si="7"/>
+        <v>147.78438600454393</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>200</v>
       </c>
@@ -3378,11 +4178,15 @@
         <v>200</v>
       </c>
       <c r="E202">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>150</v>
       </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F202">
+        <f t="shared" si="7"/>
+        <v>149.42311090716365</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>201</v>
       </c>
@@ -3393,11 +4197,15 @@
         <v>201</v>
       </c>
       <c r="E203">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>151</v>
       </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F203">
+        <f t="shared" si="7"/>
+        <v>151.0716977318159</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>202</v>
       </c>
@@ -3408,11 +4216,15 @@
         <v>202</v>
       </c>
       <c r="E204">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>153</v>
       </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F204">
+        <f t="shared" si="7"/>
+        <v>152.73015632079051</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>203</v>
       </c>
@@ -3423,11 +4235,15 @@
         <v>203</v>
       </c>
       <c r="E205">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>155</v>
       </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F205">
+        <f t="shared" si="7"/>
+        <v>154.39849647728133</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>204</v>
       </c>
@@ -3438,11 +4254,15 @@
         <v>204</v>
       </c>
       <c r="E206">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>156</v>
       </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F206">
+        <f t="shared" si="7"/>
+        <v>156.07672796573405</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>205</v>
       </c>
@@ -3453,11 +4273,15 @@
         <v>205</v>
       </c>
       <c r="E207">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>158</v>
       </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F207">
+        <f t="shared" si="7"/>
+        <v>157.76486051218879</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>206</v>
       </c>
@@ -3468,11 +4292,15 @@
         <v>206</v>
       </c>
       <c r="E208">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>160</v>
       </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F208">
+        <f t="shared" si="7"/>
+        <v>159.46290380461878</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>207</v>
       </c>
@@ -3483,11 +4311,15 @@
         <v>207</v>
       </c>
       <c r="E209">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>162</v>
       </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F209">
+        <f t="shared" si="7"/>
+        <v>161.17086749326356</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>208</v>
       </c>
@@ -3498,11 +4330,15 @@
         <v>208</v>
       </c>
       <c r="E210">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>163</v>
       </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F210">
+        <f t="shared" si="7"/>
+        <v>162.88876119095829</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>209</v>
       </c>
@@ -3513,11 +4349,15 @@
         <v>209</v>
       </c>
       <c r="E211">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>165</v>
       </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F211">
+        <f t="shared" si="7"/>
+        <v>164.61659447345829</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>210</v>
       </c>
@@ -3528,11 +4368,15 @@
         <v>210</v>
       </c>
       <c r="E212">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>167</v>
       </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F212">
+        <f t="shared" si="7"/>
+        <v>166.35437687975937</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>211</v>
       </c>
@@ -3543,11 +4387,15 @@
         <v>211</v>
       </c>
       <c r="E213">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>168</v>
       </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F213">
+        <f t="shared" si="7"/>
+        <v>168.10211791241377</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>212</v>
       </c>
@@ -3558,11 +4406,15 @@
         <v>212</v>
       </c>
       <c r="E214">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>170</v>
       </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F214">
+        <f t="shared" si="7"/>
+        <v>169.85982703784197</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>213</v>
       </c>
@@ -3573,11 +4425,15 @@
         <v>213</v>
       </c>
       <c r="E215">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>172</v>
       </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F215">
+        <f t="shared" si="7"/>
+        <v>171.62751368664019</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>214</v>
       </c>
@@ -3588,11 +4444,15 @@
         <v>214</v>
       </c>
       <c r="E216">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>174</v>
       </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F216">
+        <f t="shared" si="7"/>
+        <v>173.40518725388435</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>215</v>
       </c>
@@ -3603,11 +4463,15 @@
         <v>215</v>
       </c>
       <c r="E217">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>176</v>
       </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F217">
+        <f t="shared" si="7"/>
+        <v>175.19285709942935</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>216</v>
       </c>
@@ -3618,11 +4482,15 @@
         <v>216</v>
       </c>
       <c r="E218">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>177</v>
       </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F218">
+        <f t="shared" si="7"/>
+        <v>176.99053254820495</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>217</v>
       </c>
@@ -3633,11 +4501,15 @@
         <v>217</v>
       </c>
       <c r="E219">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>179</v>
       </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F219">
+        <f t="shared" si="7"/>
+        <v>178.79822289050753</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>218</v>
       </c>
@@ -3648,11 +4520,15 @@
         <v>218</v>
       </c>
       <c r="E220">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>181</v>
       </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F220">
+        <f t="shared" si="7"/>
+        <v>180.61593738228822</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>219</v>
       </c>
@@ -3663,11 +4539,15 @@
         <v>219</v>
       </c>
       <c r="E221">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>183</v>
       </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F221">
+        <f t="shared" si="7"/>
+        <v>182.44368524543734</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>220</v>
       </c>
@@ -3678,11 +4558,15 @@
         <v>220</v>
       </c>
       <c r="E222">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>185</v>
       </c>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F222">
+        <f t="shared" si="7"/>
+        <v>184.2814756680649</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>221</v>
       </c>
@@ -3693,11 +4577,15 @@
         <v>221</v>
       </c>
       <c r="E223">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>187</v>
       </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F223">
+        <f t="shared" si="7"/>
+        <v>186.129317804778</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>222</v>
       </c>
@@ -3708,11 +4596,15 @@
         <v>222</v>
       </c>
       <c r="E224">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>188</v>
       </c>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F224">
+        <f t="shared" si="7"/>
+        <v>187.9872207769543</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>223</v>
       </c>
@@ -3723,11 +4615,15 @@
         <v>223</v>
       </c>
       <c r="E225">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>190</v>
       </c>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F225">
+        <f t="shared" si="7"/>
+        <v>189.85519367301231</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>224</v>
       </c>
@@ -3738,11 +4634,15 @@
         <v>224</v>
       </c>
       <c r="E226">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>192</v>
       </c>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F226">
+        <f t="shared" si="7"/>
+        <v>191.73324554867798</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>225</v>
       </c>
@@ -3753,11 +4653,15 @@
         <v>225</v>
       </c>
       <c r="E227">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>193</v>
       </c>
-    </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F227">
+        <f t="shared" si="7"/>
+        <v>193.62138542724824</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>226</v>
       </c>
@@ -3768,11 +4672,15 @@
         <v>226</v>
       </c>
       <c r="E228">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>196</v>
       </c>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F228">
+        <f t="shared" si="7"/>
+        <v>195.51962229985114</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>227</v>
       </c>
@@ -3783,11 +4691,15 @@
         <v>227</v>
       </c>
       <c r="E229">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>198</v>
       </c>
-    </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F229">
+        <f t="shared" si="7"/>
+        <v>197.4279651257026</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>228</v>
       </c>
@@ -3798,11 +4710,15 @@
         <v>228</v>
       </c>
       <c r="E230">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>200</v>
       </c>
-    </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F230">
+        <f t="shared" si="7"/>
+        <v>199.34642283236039</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>229</v>
       </c>
@@ -3813,11 +4729,15 @@
         <v>229</v>
       </c>
       <c r="E231">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>202</v>
       </c>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F231">
+        <f t="shared" si="7"/>
+        <v>201.2750043159744</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>230</v>
       </c>
@@ -3828,11 +4748,15 @@
         <v>230</v>
       </c>
       <c r="E232">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>204</v>
       </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F232">
+        <f t="shared" si="7"/>
+        <v>203.21371844153441</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>231</v>
       </c>
@@ -3843,11 +4767,15 @@
         <v>231</v>
       </c>
       <c r="E233">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>206</v>
       </c>
-    </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F233">
+        <f t="shared" si="7"/>
+        <v>205.16257404311457</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>232</v>
       </c>
@@ -3858,11 +4786,15 @@
         <v>232</v>
       </c>
       <c r="E234">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>208</v>
       </c>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F234">
+        <f t="shared" si="7"/>
+        <v>207.12157992411483</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>233</v>
       </c>
@@ -3873,11 +4805,15 @@
         <v>233</v>
       </c>
       <c r="E235">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>210</v>
       </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F235">
+        <f t="shared" si="7"/>
+        <v>209.09074485749963</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>234</v>
       </c>
@@ -3888,11 +4824,15 @@
         <v>234</v>
       </c>
       <c r="E236">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>212</v>
       </c>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F236">
+        <f t="shared" si="7"/>
+        <v>211.07007758603359</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>235</v>
       </c>
@@ -3903,11 +4843,15 @@
         <v>235</v>
       </c>
       <c r="E237">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>214</v>
       </c>
-    </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F237">
+        <f t="shared" si="7"/>
+        <v>213.05958682251443</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>236</v>
       </c>
@@ -3918,11 +4862,15 @@
         <v>236</v>
       </c>
       <c r="E238">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>216</v>
       </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F238">
+        <f t="shared" si="7"/>
+        <v>215.05928125000318</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>237</v>
       </c>
@@ -3933,11 +4881,15 @@
         <v>237</v>
       </c>
       <c r="E239">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>218</v>
       </c>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F239">
+        <f t="shared" si="7"/>
+        <v>217.06916952205131</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>238</v>
       </c>
@@ -3948,11 +4900,15 @@
         <v>238</v>
       </c>
       <c r="E240">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>220</v>
       </c>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F240">
+        <f t="shared" si="7"/>
+        <v>219.08926026292573</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>239</v>
       </c>
@@ -3963,11 +4919,15 @@
         <v>239</v>
       </c>
       <c r="E241">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>222</v>
       </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F241">
+        <f t="shared" si="7"/>
+        <v>221.11956206783071</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>240</v>
       </c>
@@ -3978,11 +4938,15 @@
         <v>240</v>
       </c>
       <c r="E242">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>224</v>
       </c>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F242">
+        <f t="shared" si="7"/>
+        <v>223.16008350312725</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>241</v>
       </c>
@@ -3993,11 +4957,15 @@
         <v>241</v>
       </c>
       <c r="E243">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>226</v>
       </c>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F243">
+        <f t="shared" si="7"/>
+        <v>225.21083310655004</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>242</v>
       </c>
@@ -4008,11 +4976,15 @@
         <v>242</v>
       </c>
       <c r="E244">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>228</v>
       </c>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F244">
+        <f t="shared" si="7"/>
+        <v>227.27181938742177</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>243</v>
       </c>
@@ -4023,11 +4995,15 @@
         <v>243</v>
       </c>
       <c r="E245">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>230</v>
       </c>
-    </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F245">
+        <f t="shared" si="7"/>
+        <v>229.34305082686501</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>244</v>
       </c>
@@ -4038,11 +5014,15 @@
         <v>244</v>
       </c>
       <c r="E246">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>232</v>
       </c>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F246">
+        <f t="shared" si="7"/>
+        <v>231.42453587801157</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>245</v>
       </c>
@@ -4053,11 +5033,15 @@
         <v>245</v>
       </c>
       <c r="E247">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>234</v>
       </c>
-    </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F247">
+        <f t="shared" si="7"/>
+        <v>233.51628296620945</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>246</v>
       </c>
@@ -4068,11 +5052,15 @@
         <v>246</v>
       </c>
       <c r="E248">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>236</v>
       </c>
-    </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F248">
+        <f t="shared" si="7"/>
+        <v>235.61830048922766</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>247</v>
       </c>
@@ -4083,11 +5071,15 @@
         <v>247</v>
       </c>
       <c r="E249">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>238</v>
       </c>
-    </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F249">
+        <f t="shared" si="7"/>
+        <v>237.73059681745841</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>248</v>
       </c>
@@ -4098,11 +5090,15 @@
         <v>248</v>
       </c>
       <c r="E250">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>240</v>
       </c>
-    </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F250">
+        <f t="shared" si="7"/>
+        <v>239.85318029411704</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>249</v>
       </c>
@@ -4113,11 +5109,15 @@
         <v>249</v>
       </c>
       <c r="E251">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>243</v>
       </c>
-    </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F251">
+        <f t="shared" si="7"/>
+        <v>241.98605923543977</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>250</v>
       </c>
@@ -4128,11 +5128,15 @@
         <v>250</v>
       </c>
       <c r="E252">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>245</v>
       </c>
-    </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F252">
+        <f t="shared" si="7"/>
+        <v>244.12924193087932</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>251</v>
       </c>
@@ -4143,11 +5147,15 @@
         <v>251</v>
       </c>
       <c r="E253">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>247</v>
       </c>
-    </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F253">
+        <f t="shared" si="7"/>
+        <v>246.28273664329819</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>252</v>
       </c>
@@ -4158,11 +5166,15 @@
         <v>252</v>
       </c>
       <c r="E254">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>249</v>
       </c>
-    </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F254">
+        <f t="shared" si="7"/>
+        <v>248.44655160915963</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>253</v>
       </c>
@@ -4173,11 +5185,15 @@
         <v>253</v>
       </c>
       <c r="E255">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>251</v>
       </c>
-    </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F255">
+        <f t="shared" si="7"/>
+        <v>250.62069503871678</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>254</v>
       </c>
@@ -4188,11 +5204,15 @@
         <v>254</v>
       </c>
       <c r="E256">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>253</v>
       </c>
-    </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F256">
+        <f t="shared" si="7"/>
+        <v>252.80517511619968</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>255</v>
       </c>
@@ -4203,7 +5223,11 @@
         <v>255</v>
       </c>
       <c r="E257">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
+        <v>255</v>
+      </c>
+      <c r="F257">
+        <f t="shared" si="7"/>
         <v>255</v>
       </c>
     </row>

</xml_diff>